<commit_message>
significant updates to use Enums instead of string literals.
</commit_message>
<xml_diff>
--- a/utilityscripts/wind/as1170_2.xlsx
+++ b/utilityscripts/wind/as1170_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\wind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4BFEA-897E-43C5-A21F-4897069A4A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C320D98B-0805-4577-ADA2-C5F5F4BDE0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="68">
   <si>
     <t>N</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>f_y</t>
+  </si>
+  <si>
+    <t>AS/NZS1170.2-2011</t>
+  </si>
+  <si>
+    <t>AS/NZS1170.2-2021</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6BFCE-8807-4FA6-8CAD-90A0E49EBC9F}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3FA9CA-B7A2-4CAB-99B0-2332ACD239DB}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +994,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2011</v>
+      <c r="A2" t="s">
+        <v>66</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -999,8 +1005,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
+      <c r="A3" t="s">
+        <v>66</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1010,8 +1016,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2011</v>
+      <c r="A4" t="s">
+        <v>66</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1021,8 +1027,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2011</v>
+      <c r="A5" t="s">
+        <v>66</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1032,8 +1038,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6">
         <v>1.5</v>
@@ -1043,8 +1049,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1054,8 +1060,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2021</v>
+      <c r="A8" t="s">
+        <v>67</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1065,8 +1071,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2021</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -1117,8 +1123,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2011</v>
+      <c r="A2" t="s">
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1143,8 +1149,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
+      <c r="A3" t="s">
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1169,8 +1175,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2011</v>
+      <c r="A4" t="s">
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -1195,8 +1201,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2011</v>
+      <c r="A5" t="s">
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1221,8 +1227,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2011</v>
+      <c r="A6" t="s">
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1247,8 +1253,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2011</v>
+      <c r="A7" t="s">
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -1273,8 +1279,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2011</v>
+      <c r="A8" t="s">
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1299,8 +1305,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2011</v>
+      <c r="A9" t="s">
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1325,8 +1331,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2011</v>
+      <c r="A10" t="s">
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1351,8 +1357,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2011</v>
+      <c r="A11" t="s">
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -1377,8 +1383,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2011</v>
+      <c r="A12" t="s">
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -1403,8 +1409,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
+      <c r="A13" t="s">
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -1429,8 +1435,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2021</v>
+      <c r="A14" t="s">
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -1455,8 +1461,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2021</v>
+      <c r="A15" t="s">
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1481,8 +1487,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2021</v>
+      <c r="A16" t="s">
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1507,8 +1513,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2021</v>
+      <c r="A17" t="s">
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1533,8 +1539,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2021</v>
+      <c r="A18" t="s">
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1559,8 +1565,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2021</v>
+      <c r="A19" t="s">
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -1585,8 +1591,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2021</v>
+      <c r="A20" t="s">
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -1611,8 +1617,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2021</v>
+      <c r="A21" t="s">
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -1637,8 +1643,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2021</v>
+      <c r="A22" t="s">
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -1663,8 +1669,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2021</v>
+      <c r="A23" t="s">
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -1689,8 +1695,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2021</v>
+      <c r="A24" t="s">
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
@@ -1715,8 +1721,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2021</v>
+      <c r="A25" t="s">
+        <v>67</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
@@ -1741,8 +1747,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2021</v>
+      <c r="A26" t="s">
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -1776,7 +1782,7 @@
   <dimension ref="A1:D251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,8 +1808,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2011</v>
+      <c r="A2" t="s">
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1816,8 +1822,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
+      <c r="A3" t="s">
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1830,8 +1836,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2011</v>
+      <c r="A4" t="s">
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -1844,8 +1850,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2011</v>
+      <c r="A5" t="s">
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -1858,8 +1864,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2011</v>
+      <c r="A6" t="s">
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1872,8 +1878,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2011</v>
+      <c r="A7" t="s">
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1886,8 +1892,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2011</v>
+      <c r="A8" t="s">
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1900,8 +1906,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2011</v>
+      <c r="A9" t="s">
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1914,8 +1920,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2011</v>
+      <c r="A10" t="s">
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1928,8 +1934,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2011</v>
+      <c r="A11" t="s">
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -1942,8 +1948,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2011</v>
+      <c r="A12" t="s">
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1956,8 +1962,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2011</v>
+      <c r="A13" t="s">
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1970,8 +1976,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2011</v>
+      <c r="A14" t="s">
+        <v>66</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -1984,8 +1990,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2011</v>
+      <c r="A15" t="s">
+        <v>66</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -1998,8 +2004,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2011</v>
+      <c r="A16" t="s">
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -2012,8 +2018,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2011</v>
+      <c r="A17" t="s">
+        <v>66</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -2026,8 +2032,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2011</v>
+      <c r="A18" t="s">
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -2040,8 +2046,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2011</v>
+      <c r="A19" t="s">
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -2054,8 +2060,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2011</v>
+      <c r="A20" t="s">
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -2068,8 +2074,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2011</v>
+      <c r="A21" t="s">
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -2082,8 +2088,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2011</v>
+      <c r="A22" t="s">
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -2096,8 +2102,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2011</v>
+      <c r="A23" t="s">
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -2110,8 +2116,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2011</v>
+      <c r="A24" t="s">
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
@@ -2124,8 +2130,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2011</v>
+      <c r="A25" t="s">
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -2138,8 +2144,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2011</v>
+      <c r="A26" t="s">
+        <v>66</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
@@ -2152,8 +2158,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2011</v>
+      <c r="A27" t="s">
+        <v>66</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -2166,8 +2172,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2011</v>
+      <c r="A28" t="s">
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -2180,8 +2186,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2011</v>
+      <c r="A29" t="s">
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
@@ -2194,8 +2200,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2011</v>
+      <c r="A30" t="s">
+        <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
@@ -2208,8 +2214,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2011</v>
+      <c r="A31" t="s">
+        <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -2222,8 +2228,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2011</v>
+      <c r="A32" t="s">
+        <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -2236,8 +2242,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2011</v>
+      <c r="A33" t="s">
+        <v>66</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -2250,8 +2256,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2011</v>
+      <c r="A34" t="s">
+        <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -2264,8 +2270,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2011</v>
+      <c r="A35" t="s">
+        <v>66</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -2278,8 +2284,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2011</v>
+      <c r="A36" t="s">
+        <v>66</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
@@ -2292,8 +2298,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2011</v>
+      <c r="A37" t="s">
+        <v>66</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
@@ -2306,8 +2312,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2011</v>
+      <c r="A38" t="s">
+        <v>66</v>
       </c>
       <c r="B38" t="s">
         <v>16</v>
@@ -2320,8 +2326,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2011</v>
+      <c r="A39" t="s">
+        <v>66</v>
       </c>
       <c r="B39" t="s">
         <v>16</v>
@@ -2334,8 +2340,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2011</v>
+      <c r="A40" t="s">
+        <v>66</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -2348,8 +2354,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2011</v>
+      <c r="A41" t="s">
+        <v>66</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -2362,8 +2368,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2011</v>
+      <c r="A42" t="s">
+        <v>66</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
@@ -2376,8 +2382,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2011</v>
+      <c r="A43" t="s">
+        <v>66</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -2390,8 +2396,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2011</v>
+      <c r="A44" t="s">
+        <v>66</v>
       </c>
       <c r="B44" t="s">
         <v>17</v>
@@ -2404,8 +2410,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2011</v>
+      <c r="A45" t="s">
+        <v>66</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
@@ -2418,8 +2424,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2011</v>
+      <c r="A46" t="s">
+        <v>66</v>
       </c>
       <c r="B46" t="s">
         <v>17</v>
@@ -2432,8 +2438,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2011</v>
+      <c r="A47" t="s">
+        <v>66</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -2446,8 +2452,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2011</v>
+      <c r="A48" t="s">
+        <v>66</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -2460,8 +2466,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2011</v>
+      <c r="A49" t="s">
+        <v>66</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
@@ -2474,8 +2480,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2011</v>
+      <c r="A50" t="s">
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -2488,8 +2494,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>2011</v>
+      <c r="A51" t="s">
+        <v>66</v>
       </c>
       <c r="B51" t="s">
         <v>17</v>
@@ -2502,8 +2508,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2011</v>
+      <c r="A52" t="s">
+        <v>66</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
@@ -2516,8 +2522,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2011</v>
+      <c r="A53" t="s">
+        <v>66</v>
       </c>
       <c r="B53" t="s">
         <v>18</v>
@@ -2530,8 +2536,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>2011</v>
+      <c r="A54" t="s">
+        <v>66</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
@@ -2544,8 +2550,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>2011</v>
+      <c r="A55" t="s">
+        <v>66</v>
       </c>
       <c r="B55" t="s">
         <v>18</v>
@@ -2558,8 +2564,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>2011</v>
+      <c r="A56" t="s">
+        <v>66</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
@@ -2572,8 +2578,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>2011</v>
+      <c r="A57" t="s">
+        <v>66</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
@@ -2586,8 +2592,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>2011</v>
+      <c r="A58" t="s">
+        <v>66</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -2600,8 +2606,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2011</v>
+      <c r="A59" t="s">
+        <v>66</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
@@ -2614,8 +2620,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>2011</v>
+      <c r="A60" t="s">
+        <v>66</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -2628,8 +2634,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2011</v>
+      <c r="A61" t="s">
+        <v>66</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
@@ -2642,8 +2648,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>2011</v>
+      <c r="A62" t="s">
+        <v>66</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
@@ -2656,8 +2662,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>2011</v>
+      <c r="A63" t="s">
+        <v>66</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
@@ -2670,8 +2676,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2011</v>
+      <c r="A64" t="s">
+        <v>66</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
@@ -2684,8 +2690,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>2011</v>
+      <c r="A65" t="s">
+        <v>66</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
@@ -2698,8 +2704,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>2011</v>
+      <c r="A66" t="s">
+        <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
@@ -2712,8 +2718,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>2011</v>
+      <c r="A67" t="s">
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>19</v>
@@ -2726,8 +2732,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>2011</v>
+      <c r="A68" t="s">
+        <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
@@ -2740,8 +2746,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>2011</v>
+      <c r="A69" t="s">
+        <v>66</v>
       </c>
       <c r="B69" t="s">
         <v>19</v>
@@ -2754,8 +2760,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>2011</v>
+      <c r="A70" t="s">
+        <v>66</v>
       </c>
       <c r="B70" t="s">
         <v>19</v>
@@ -2768,8 +2774,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>2011</v>
+      <c r="A71" t="s">
+        <v>66</v>
       </c>
       <c r="B71" t="s">
         <v>19</v>
@@ -2782,8 +2788,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>2011</v>
+      <c r="A72" t="s">
+        <v>66</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -2796,8 +2802,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>2011</v>
+      <c r="A73" t="s">
+        <v>66</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -2810,8 +2816,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>2011</v>
+      <c r="A74" t="s">
+        <v>66</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -2824,8 +2830,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>2011</v>
+      <c r="A75" t="s">
+        <v>66</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -2838,8 +2844,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>2011</v>
+      <c r="A76" t="s">
+        <v>66</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -2852,8 +2858,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>2011</v>
+      <c r="A77" t="s">
+        <v>66</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -2866,8 +2872,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>2011</v>
+      <c r="A78" t="s">
+        <v>66</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -2880,8 +2886,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>2011</v>
+      <c r="A79" t="s">
+        <v>66</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -2894,8 +2900,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>2011</v>
+      <c r="A80" t="s">
+        <v>66</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -2908,8 +2914,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>2011</v>
+      <c r="A81" t="s">
+        <v>66</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
@@ -2922,8 +2928,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>2011</v>
+      <c r="A82" t="s">
+        <v>66</v>
       </c>
       <c r="B82" t="s">
         <v>20</v>
@@ -2936,8 +2942,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>2011</v>
+      <c r="A83" t="s">
+        <v>66</v>
       </c>
       <c r="B83" t="s">
         <v>20</v>
@@ -2950,8 +2956,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>2011</v>
+      <c r="A84" t="s">
+        <v>66</v>
       </c>
       <c r="B84" t="s">
         <v>20</v>
@@ -2964,8 +2970,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>2011</v>
+      <c r="A85" t="s">
+        <v>66</v>
       </c>
       <c r="B85" t="s">
         <v>20</v>
@@ -2978,8 +2984,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>2011</v>
+      <c r="A86" t="s">
+        <v>66</v>
       </c>
       <c r="B86" t="s">
         <v>20</v>
@@ -2992,8 +2998,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>2011</v>
+      <c r="A87" t="s">
+        <v>66</v>
       </c>
       <c r="B87" t="s">
         <v>20</v>
@@ -3006,8 +3012,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>2011</v>
+      <c r="A88" t="s">
+        <v>66</v>
       </c>
       <c r="B88" t="s">
         <v>20</v>
@@ -3020,8 +3026,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>2011</v>
+      <c r="A89" t="s">
+        <v>66</v>
       </c>
       <c r="B89" t="s">
         <v>20</v>
@@ -3034,8 +3040,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>2011</v>
+      <c r="A90" t="s">
+        <v>66</v>
       </c>
       <c r="B90" t="s">
         <v>20</v>
@@ -3048,8 +3054,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>2011</v>
+      <c r="A91" t="s">
+        <v>66</v>
       </c>
       <c r="B91" t="s">
         <v>20</v>
@@ -3062,8 +3068,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>2011</v>
+      <c r="A92" t="s">
+        <v>66</v>
       </c>
       <c r="B92" t="s">
         <v>21</v>
@@ -3076,8 +3082,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>2011</v>
+      <c r="A93" t="s">
+        <v>66</v>
       </c>
       <c r="B93" t="s">
         <v>21</v>
@@ -3090,8 +3096,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>2011</v>
+      <c r="A94" t="s">
+        <v>66</v>
       </c>
       <c r="B94" t="s">
         <v>21</v>
@@ -3104,8 +3110,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2011</v>
+      <c r="A95" t="s">
+        <v>66</v>
       </c>
       <c r="B95" t="s">
         <v>21</v>
@@ -3118,8 +3124,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>2011</v>
+      <c r="A96" t="s">
+        <v>66</v>
       </c>
       <c r="B96" t="s">
         <v>21</v>
@@ -3132,8 +3138,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>2011</v>
+      <c r="A97" t="s">
+        <v>66</v>
       </c>
       <c r="B97" t="s">
         <v>21</v>
@@ -3146,8 +3152,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>2011</v>
+      <c r="A98" t="s">
+        <v>66</v>
       </c>
       <c r="B98" t="s">
         <v>21</v>
@@ -3160,8 +3166,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>2011</v>
+      <c r="A99" t="s">
+        <v>66</v>
       </c>
       <c r="B99" t="s">
         <v>21</v>
@@ -3174,8 +3180,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>2011</v>
+      <c r="A100" t="s">
+        <v>66</v>
       </c>
       <c r="B100" t="s">
         <v>21</v>
@@ -3188,8 +3194,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>2011</v>
+      <c r="A101" t="s">
+        <v>66</v>
       </c>
       <c r="B101" t="s">
         <v>21</v>
@@ -3202,8 +3208,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>2011</v>
+      <c r="A102" t="s">
+        <v>66</v>
       </c>
       <c r="B102" t="s">
         <v>22</v>
@@ -3216,8 +3222,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>2011</v>
+      <c r="A103" t="s">
+        <v>66</v>
       </c>
       <c r="B103" t="s">
         <v>22</v>
@@ -3230,8 +3236,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>2011</v>
+      <c r="A104" t="s">
+        <v>66</v>
       </c>
       <c r="B104" t="s">
         <v>22</v>
@@ -3244,8 +3250,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>2011</v>
+      <c r="A105" t="s">
+        <v>66</v>
       </c>
       <c r="B105" t="s">
         <v>22</v>
@@ -3258,8 +3264,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>2011</v>
+      <c r="A106" t="s">
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>22</v>
@@ -3272,8 +3278,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>2011</v>
+      <c r="A107" t="s">
+        <v>66</v>
       </c>
       <c r="B107" t="s">
         <v>22</v>
@@ -3286,8 +3292,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>2011</v>
+      <c r="A108" t="s">
+        <v>66</v>
       </c>
       <c r="B108" t="s">
         <v>22</v>
@@ -3300,8 +3306,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>2011</v>
+      <c r="A109" t="s">
+        <v>66</v>
       </c>
       <c r="B109" t="s">
         <v>22</v>
@@ -3314,8 +3320,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>2011</v>
+      <c r="A110" t="s">
+        <v>66</v>
       </c>
       <c r="B110" t="s">
         <v>22</v>
@@ -3328,8 +3334,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>2011</v>
+      <c r="A111" t="s">
+        <v>66</v>
       </c>
       <c r="B111" t="s">
         <v>22</v>
@@ -3342,8 +3348,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>2021</v>
+      <c r="A112" t="s">
+        <v>67</v>
       </c>
       <c r="B112" t="s">
         <v>23</v>
@@ -3356,8 +3362,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>2021</v>
+      <c r="A113" t="s">
+        <v>67</v>
       </c>
       <c r="B113" t="s">
         <v>23</v>
@@ -3370,8 +3376,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>2021</v>
+      <c r="A114" t="s">
+        <v>67</v>
       </c>
       <c r="B114" t="s">
         <v>23</v>
@@ -3384,8 +3390,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>2021</v>
+      <c r="A115" t="s">
+        <v>67</v>
       </c>
       <c r="B115" t="s">
         <v>23</v>
@@ -3398,8 +3404,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>2021</v>
+      <c r="A116" t="s">
+        <v>67</v>
       </c>
       <c r="B116" t="s">
         <v>23</v>
@@ -3412,8 +3418,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>2021</v>
+      <c r="A117" t="s">
+        <v>67</v>
       </c>
       <c r="B117" t="s">
         <v>23</v>
@@ -3426,8 +3432,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>2021</v>
+      <c r="A118" t="s">
+        <v>67</v>
       </c>
       <c r="B118" t="s">
         <v>23</v>
@@ -3440,8 +3446,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>2021</v>
+      <c r="A119" t="s">
+        <v>67</v>
       </c>
       <c r="B119" t="s">
         <v>23</v>
@@ -3454,8 +3460,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>2021</v>
+      <c r="A120" t="s">
+        <v>67</v>
       </c>
       <c r="B120" t="s">
         <v>23</v>
@@ -3468,8 +3474,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>2021</v>
+      <c r="A121" t="s">
+        <v>67</v>
       </c>
       <c r="B121" t="s">
         <v>23</v>
@@ -3482,8 +3488,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>2021</v>
+      <c r="A122" t="s">
+        <v>67</v>
       </c>
       <c r="B122" t="s">
         <v>13</v>
@@ -3496,8 +3502,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>2021</v>
+      <c r="A123" t="s">
+        <v>67</v>
       </c>
       <c r="B123" t="s">
         <v>13</v>
@@ -3510,8 +3516,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>2021</v>
+      <c r="A124" t="s">
+        <v>67</v>
       </c>
       <c r="B124" t="s">
         <v>13</v>
@@ -3524,8 +3530,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>2021</v>
+      <c r="A125" t="s">
+        <v>67</v>
       </c>
       <c r="B125" t="s">
         <v>13</v>
@@ -3538,8 +3544,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>2021</v>
+      <c r="A126" t="s">
+        <v>67</v>
       </c>
       <c r="B126" t="s">
         <v>13</v>
@@ -3552,8 +3558,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>2021</v>
+      <c r="A127" t="s">
+        <v>67</v>
       </c>
       <c r="B127" t="s">
         <v>13</v>
@@ -3566,8 +3572,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>2021</v>
+      <c r="A128" t="s">
+        <v>67</v>
       </c>
       <c r="B128" t="s">
         <v>13</v>
@@ -3580,8 +3586,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>2021</v>
+      <c r="A129" t="s">
+        <v>67</v>
       </c>
       <c r="B129" t="s">
         <v>13</v>
@@ -3594,8 +3600,8 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>2021</v>
+      <c r="A130" t="s">
+        <v>67</v>
       </c>
       <c r="B130" t="s">
         <v>13</v>
@@ -3608,8 +3614,8 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131">
-        <v>2021</v>
+      <c r="A131" t="s">
+        <v>67</v>
       </c>
       <c r="B131" t="s">
         <v>13</v>
@@ -3622,8 +3628,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132">
-        <v>2021</v>
+      <c r="A132" t="s">
+        <v>67</v>
       </c>
       <c r="B132" t="s">
         <v>14</v>
@@ -3636,8 +3642,8 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>2021</v>
+      <c r="A133" t="s">
+        <v>67</v>
       </c>
       <c r="B133" t="s">
         <v>14</v>
@@ -3650,8 +3656,8 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>2021</v>
+      <c r="A134" t="s">
+        <v>67</v>
       </c>
       <c r="B134" t="s">
         <v>14</v>
@@ -3664,8 +3670,8 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135">
-        <v>2021</v>
+      <c r="A135" t="s">
+        <v>67</v>
       </c>
       <c r="B135" t="s">
         <v>14</v>
@@ -3678,8 +3684,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136">
-        <v>2021</v>
+      <c r="A136" t="s">
+        <v>67</v>
       </c>
       <c r="B136" t="s">
         <v>14</v>
@@ -3692,8 +3698,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>2021</v>
+      <c r="A137" t="s">
+        <v>67</v>
       </c>
       <c r="B137" t="s">
         <v>14</v>
@@ -3706,8 +3712,8 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138">
-        <v>2021</v>
+      <c r="A138" t="s">
+        <v>67</v>
       </c>
       <c r="B138" t="s">
         <v>14</v>
@@ -3720,8 +3726,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>2021</v>
+      <c r="A139" t="s">
+        <v>67</v>
       </c>
       <c r="B139" t="s">
         <v>14</v>
@@ -3734,8 +3740,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>2021</v>
+      <c r="A140" t="s">
+        <v>67</v>
       </c>
       <c r="B140" t="s">
         <v>14</v>
@@ -3748,8 +3754,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>2021</v>
+      <c r="A141" t="s">
+        <v>67</v>
       </c>
       <c r="B141" t="s">
         <v>14</v>
@@ -3762,8 +3768,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>2021</v>
+      <c r="A142" t="s">
+        <v>67</v>
       </c>
       <c r="B142" t="s">
         <v>15</v>
@@ -3776,8 +3782,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>2021</v>
+      <c r="A143" t="s">
+        <v>67</v>
       </c>
       <c r="B143" t="s">
         <v>15</v>
@@ -3790,8 +3796,8 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>2021</v>
+      <c r="A144" t="s">
+        <v>67</v>
       </c>
       <c r="B144" t="s">
         <v>15</v>
@@ -3804,8 +3810,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>2021</v>
+      <c r="A145" t="s">
+        <v>67</v>
       </c>
       <c r="B145" t="s">
         <v>15</v>
@@ -3818,8 +3824,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>2021</v>
+      <c r="A146" t="s">
+        <v>67</v>
       </c>
       <c r="B146" t="s">
         <v>15</v>
@@ -3832,8 +3838,8 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>2021</v>
+      <c r="A147" t="s">
+        <v>67</v>
       </c>
       <c r="B147" t="s">
         <v>15</v>
@@ -3846,8 +3852,8 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>2021</v>
+      <c r="A148" t="s">
+        <v>67</v>
       </c>
       <c r="B148" t="s">
         <v>15</v>
@@ -3860,8 +3866,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>2021</v>
+      <c r="A149" t="s">
+        <v>67</v>
       </c>
       <c r="B149" t="s">
         <v>15</v>
@@ -3874,8 +3880,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>2021</v>
+      <c r="A150" t="s">
+        <v>67</v>
       </c>
       <c r="B150" t="s">
         <v>15</v>
@@ -3888,8 +3894,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>2021</v>
+      <c r="A151" t="s">
+        <v>67</v>
       </c>
       <c r="B151" t="s">
         <v>15</v>
@@ -3902,8 +3908,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>2021</v>
+      <c r="A152" t="s">
+        <v>67</v>
       </c>
       <c r="B152" t="s">
         <v>16</v>
@@ -3916,8 +3922,8 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>2021</v>
+      <c r="A153" t="s">
+        <v>67</v>
       </c>
       <c r="B153" t="s">
         <v>16</v>
@@ -3930,8 +3936,8 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154">
-        <v>2021</v>
+      <c r="A154" t="s">
+        <v>67</v>
       </c>
       <c r="B154" t="s">
         <v>16</v>
@@ -3944,8 +3950,8 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>2021</v>
+      <c r="A155" t="s">
+        <v>67</v>
       </c>
       <c r="B155" t="s">
         <v>16</v>
@@ -3958,8 +3964,8 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156">
-        <v>2021</v>
+      <c r="A156" t="s">
+        <v>67</v>
       </c>
       <c r="B156" t="s">
         <v>16</v>
@@ -3972,8 +3978,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157">
-        <v>2021</v>
+      <c r="A157" t="s">
+        <v>67</v>
       </c>
       <c r="B157" t="s">
         <v>16</v>
@@ -3986,8 +3992,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158">
-        <v>2021</v>
+      <c r="A158" t="s">
+        <v>67</v>
       </c>
       <c r="B158" t="s">
         <v>16</v>
@@ -4000,8 +4006,8 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159">
-        <v>2021</v>
+      <c r="A159" t="s">
+        <v>67</v>
       </c>
       <c r="B159" t="s">
         <v>16</v>
@@ -4014,8 +4020,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>2021</v>
+      <c r="A160" t="s">
+        <v>67</v>
       </c>
       <c r="B160" t="s">
         <v>16</v>
@@ -4028,8 +4034,8 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>2021</v>
+      <c r="A161" t="s">
+        <v>67</v>
       </c>
       <c r="B161" t="s">
         <v>16</v>
@@ -4042,8 +4048,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162">
-        <v>2021</v>
+      <c r="A162" t="s">
+        <v>67</v>
       </c>
       <c r="B162" t="s">
         <v>17</v>
@@ -4056,8 +4062,8 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163">
-        <v>2021</v>
+      <c r="A163" t="s">
+        <v>67</v>
       </c>
       <c r="B163" t="s">
         <v>17</v>
@@ -4070,8 +4076,8 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164">
-        <v>2021</v>
+      <c r="A164" t="s">
+        <v>67</v>
       </c>
       <c r="B164" t="s">
         <v>17</v>
@@ -4084,8 +4090,8 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>2021</v>
+      <c r="A165" t="s">
+        <v>67</v>
       </c>
       <c r="B165" t="s">
         <v>17</v>
@@ -4098,8 +4104,8 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166">
-        <v>2021</v>
+      <c r="A166" t="s">
+        <v>67</v>
       </c>
       <c r="B166" t="s">
         <v>17</v>
@@ -4112,8 +4118,8 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167">
-        <v>2021</v>
+      <c r="A167" t="s">
+        <v>67</v>
       </c>
       <c r="B167" t="s">
         <v>17</v>
@@ -4126,8 +4132,8 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>2021</v>
+      <c r="A168" t="s">
+        <v>67</v>
       </c>
       <c r="B168" t="s">
         <v>17</v>
@@ -4140,8 +4146,8 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>2021</v>
+      <c r="A169" t="s">
+        <v>67</v>
       </c>
       <c r="B169" t="s">
         <v>17</v>
@@ -4154,8 +4160,8 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170">
-        <v>2021</v>
+      <c r="A170" t="s">
+        <v>67</v>
       </c>
       <c r="B170" t="s">
         <v>17</v>
@@ -4168,8 +4174,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171">
-        <v>2021</v>
+      <c r="A171" t="s">
+        <v>67</v>
       </c>
       <c r="B171" t="s">
         <v>17</v>
@@ -4182,8 +4188,8 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172">
-        <v>2021</v>
+      <c r="A172" t="s">
+        <v>67</v>
       </c>
       <c r="B172" t="s">
         <v>24</v>
@@ -4196,8 +4202,8 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173">
-        <v>2021</v>
+      <c r="A173" t="s">
+        <v>67</v>
       </c>
       <c r="B173" t="s">
         <v>24</v>
@@ -4210,8 +4216,8 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174">
-        <v>2021</v>
+      <c r="A174" t="s">
+        <v>67</v>
       </c>
       <c r="B174" t="s">
         <v>24</v>
@@ -4224,8 +4230,8 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175">
-        <v>2021</v>
+      <c r="A175" t="s">
+        <v>67</v>
       </c>
       <c r="B175" t="s">
         <v>24</v>
@@ -4238,8 +4244,8 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>2021</v>
+      <c r="A176" t="s">
+        <v>67</v>
       </c>
       <c r="B176" t="s">
         <v>24</v>
@@ -4252,8 +4258,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177">
-        <v>2021</v>
+      <c r="A177" t="s">
+        <v>67</v>
       </c>
       <c r="B177" t="s">
         <v>24</v>
@@ -4266,8 +4272,8 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178">
-        <v>2021</v>
+      <c r="A178" t="s">
+        <v>67</v>
       </c>
       <c r="B178" t="s">
         <v>24</v>
@@ -4280,8 +4286,8 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179">
-        <v>2021</v>
+      <c r="A179" t="s">
+        <v>67</v>
       </c>
       <c r="B179" t="s">
         <v>24</v>
@@ -4294,8 +4300,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180">
-        <v>2021</v>
+      <c r="A180" t="s">
+        <v>67</v>
       </c>
       <c r="B180" t="s">
         <v>24</v>
@@ -4308,8 +4314,8 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181">
-        <v>2021</v>
+      <c r="A181" t="s">
+        <v>67</v>
       </c>
       <c r="B181" t="s">
         <v>24</v>
@@ -4322,8 +4328,8 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182">
-        <v>2021</v>
+      <c r="A182" t="s">
+        <v>67</v>
       </c>
       <c r="B182" t="s">
         <v>25</v>
@@ -4336,8 +4342,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183">
-        <v>2021</v>
+      <c r="A183" t="s">
+        <v>67</v>
       </c>
       <c r="B183" t="s">
         <v>25</v>
@@ -4350,8 +4356,8 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184">
-        <v>2021</v>
+      <c r="A184" t="s">
+        <v>67</v>
       </c>
       <c r="B184" t="s">
         <v>25</v>
@@ -4364,8 +4370,8 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185">
-        <v>2021</v>
+      <c r="A185" t="s">
+        <v>67</v>
       </c>
       <c r="B185" t="s">
         <v>25</v>
@@ -4378,8 +4384,8 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186">
-        <v>2021</v>
+      <c r="A186" t="s">
+        <v>67</v>
       </c>
       <c r="B186" t="s">
         <v>25</v>
@@ -4392,8 +4398,8 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>2021</v>
+      <c r="A187" t="s">
+        <v>67</v>
       </c>
       <c r="B187" t="s">
         <v>25</v>
@@ -4406,8 +4412,8 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188">
-        <v>2021</v>
+      <c r="A188" t="s">
+        <v>67</v>
       </c>
       <c r="B188" t="s">
         <v>25</v>
@@ -4420,8 +4426,8 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189">
-        <v>2021</v>
+      <c r="A189" t="s">
+        <v>67</v>
       </c>
       <c r="B189" t="s">
         <v>25</v>
@@ -4434,8 +4440,8 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190">
-        <v>2021</v>
+      <c r="A190" t="s">
+        <v>67</v>
       </c>
       <c r="B190" t="s">
         <v>25</v>
@@ -4448,8 +4454,8 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191">
-        <v>2021</v>
+      <c r="A191" t="s">
+        <v>67</v>
       </c>
       <c r="B191" t="s">
         <v>25</v>
@@ -4462,8 +4468,8 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192">
-        <v>2021</v>
+      <c r="A192" t="s">
+        <v>67</v>
       </c>
       <c r="B192" t="s">
         <v>21</v>
@@ -4476,8 +4482,8 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>2021</v>
+      <c r="A193" t="s">
+        <v>67</v>
       </c>
       <c r="B193" t="s">
         <v>21</v>
@@ -4490,8 +4496,8 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194">
-        <v>2021</v>
+      <c r="A194" t="s">
+        <v>67</v>
       </c>
       <c r="B194" t="s">
         <v>21</v>
@@ -4504,8 +4510,8 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195">
-        <v>2021</v>
+      <c r="A195" t="s">
+        <v>67</v>
       </c>
       <c r="B195" t="s">
         <v>21</v>
@@ -4518,8 +4524,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196">
-        <v>2021</v>
+      <c r="A196" t="s">
+        <v>67</v>
       </c>
       <c r="B196" t="s">
         <v>21</v>
@@ -4532,8 +4538,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197">
-        <v>2021</v>
+      <c r="A197" t="s">
+        <v>67</v>
       </c>
       <c r="B197" t="s">
         <v>21</v>
@@ -4546,8 +4552,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198">
-        <v>2021</v>
+      <c r="A198" t="s">
+        <v>67</v>
       </c>
       <c r="B198" t="s">
         <v>21</v>
@@ -4560,8 +4566,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199">
-        <v>2021</v>
+      <c r="A199" t="s">
+        <v>67</v>
       </c>
       <c r="B199" t="s">
         <v>21</v>
@@ -4574,8 +4580,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200">
-        <v>2021</v>
+      <c r="A200" t="s">
+        <v>67</v>
       </c>
       <c r="B200" t="s">
         <v>21</v>
@@ -4588,8 +4594,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201">
-        <v>2021</v>
+      <c r="A201" t="s">
+        <v>67</v>
       </c>
       <c r="B201" t="s">
         <v>21</v>
@@ -4602,8 +4608,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202">
-        <v>2021</v>
+      <c r="A202" t="s">
+        <v>67</v>
       </c>
       <c r="B202" t="s">
         <v>22</v>
@@ -4616,8 +4622,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203">
-        <v>2021</v>
+      <c r="A203" t="s">
+        <v>67</v>
       </c>
       <c r="B203" t="s">
         <v>22</v>
@@ -4630,8 +4636,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204">
-        <v>2021</v>
+      <c r="A204" t="s">
+        <v>67</v>
       </c>
       <c r="B204" t="s">
         <v>22</v>
@@ -4644,8 +4650,8 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205">
-        <v>2021</v>
+      <c r="A205" t="s">
+        <v>67</v>
       </c>
       <c r="B205" t="s">
         <v>22</v>
@@ -4658,8 +4664,8 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206">
-        <v>2021</v>
+      <c r="A206" t="s">
+        <v>67</v>
       </c>
       <c r="B206" t="s">
         <v>22</v>
@@ -4672,8 +4678,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207">
-        <v>2021</v>
+      <c r="A207" t="s">
+        <v>67</v>
       </c>
       <c r="B207" t="s">
         <v>22</v>
@@ -4686,8 +4692,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>2021</v>
+      <c r="A208" t="s">
+        <v>67</v>
       </c>
       <c r="B208" t="s">
         <v>22</v>
@@ -4700,8 +4706,8 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>2021</v>
+      <c r="A209" t="s">
+        <v>67</v>
       </c>
       <c r="B209" t="s">
         <v>22</v>
@@ -4714,8 +4720,8 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210">
-        <v>2021</v>
+      <c r="A210" t="s">
+        <v>67</v>
       </c>
       <c r="B210" t="s">
         <v>22</v>
@@ -4728,8 +4734,8 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211">
-        <v>2021</v>
+      <c r="A211" t="s">
+        <v>67</v>
       </c>
       <c r="B211" t="s">
         <v>22</v>
@@ -4742,8 +4748,8 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212">
-        <v>2021</v>
+      <c r="A212" t="s">
+        <v>67</v>
       </c>
       <c r="B212" t="s">
         <v>26</v>
@@ -4756,8 +4762,8 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213">
-        <v>2021</v>
+      <c r="A213" t="s">
+        <v>67</v>
       </c>
       <c r="B213" t="s">
         <v>26</v>
@@ -4770,8 +4776,8 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214">
-        <v>2021</v>
+      <c r="A214" t="s">
+        <v>67</v>
       </c>
       <c r="B214" t="s">
         <v>26</v>
@@ -4784,8 +4790,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215">
-        <v>2021</v>
+      <c r="A215" t="s">
+        <v>67</v>
       </c>
       <c r="B215" t="s">
         <v>26</v>
@@ -4798,8 +4804,8 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216">
-        <v>2021</v>
+      <c r="A216" t="s">
+        <v>67</v>
       </c>
       <c r="B216" t="s">
         <v>26</v>
@@ -4812,8 +4818,8 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217">
-        <v>2021</v>
+      <c r="A217" t="s">
+        <v>67</v>
       </c>
       <c r="B217" t="s">
         <v>26</v>
@@ -4826,8 +4832,8 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218">
-        <v>2021</v>
+      <c r="A218" t="s">
+        <v>67</v>
       </c>
       <c r="B218" t="s">
         <v>26</v>
@@ -4840,8 +4846,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219">
-        <v>2021</v>
+      <c r="A219" t="s">
+        <v>67</v>
       </c>
       <c r="B219" t="s">
         <v>26</v>
@@ -4854,8 +4860,8 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220">
-        <v>2021</v>
+      <c r="A220" t="s">
+        <v>67</v>
       </c>
       <c r="B220" t="s">
         <v>26</v>
@@ -4868,8 +4874,8 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221">
-        <v>2021</v>
+      <c r="A221" t="s">
+        <v>67</v>
       </c>
       <c r="B221" t="s">
         <v>26</v>
@@ -4882,8 +4888,8 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222">
-        <v>2021</v>
+      <c r="A222" t="s">
+        <v>67</v>
       </c>
       <c r="B222" t="s">
         <v>27</v>
@@ -4896,8 +4902,8 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223">
-        <v>2021</v>
+      <c r="A223" t="s">
+        <v>67</v>
       </c>
       <c r="B223" t="s">
         <v>27</v>
@@ -4910,8 +4916,8 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224">
-        <v>2021</v>
+      <c r="A224" t="s">
+        <v>67</v>
       </c>
       <c r="B224" t="s">
         <v>27</v>
@@ -4924,8 +4930,8 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225">
-        <v>2021</v>
+      <c r="A225" t="s">
+        <v>67</v>
       </c>
       <c r="B225" t="s">
         <v>27</v>
@@ -4938,8 +4944,8 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226">
-        <v>2021</v>
+      <c r="A226" t="s">
+        <v>67</v>
       </c>
       <c r="B226" t="s">
         <v>27</v>
@@ -4952,8 +4958,8 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227">
-        <v>2021</v>
+      <c r="A227" t="s">
+        <v>67</v>
       </c>
       <c r="B227" t="s">
         <v>27</v>
@@ -4966,8 +4972,8 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228">
-        <v>2021</v>
+      <c r="A228" t="s">
+        <v>67</v>
       </c>
       <c r="B228" t="s">
         <v>27</v>
@@ -4980,8 +4986,8 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229">
-        <v>2021</v>
+      <c r="A229" t="s">
+        <v>67</v>
       </c>
       <c r="B229" t="s">
         <v>27</v>
@@ -4994,8 +5000,8 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230">
-        <v>2021</v>
+      <c r="A230" t="s">
+        <v>67</v>
       </c>
       <c r="B230" t="s">
         <v>27</v>
@@ -5008,8 +5014,8 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231">
-        <v>2021</v>
+      <c r="A231" t="s">
+        <v>67</v>
       </c>
       <c r="B231" t="s">
         <v>27</v>
@@ -5022,8 +5028,8 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232">
-        <v>2021</v>
+      <c r="A232" t="s">
+        <v>67</v>
       </c>
       <c r="B232" t="s">
         <v>28</v>
@@ -5036,8 +5042,8 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233">
-        <v>2021</v>
+      <c r="A233" t="s">
+        <v>67</v>
       </c>
       <c r="B233" t="s">
         <v>28</v>
@@ -5050,8 +5056,8 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234">
-        <v>2021</v>
+      <c r="A234" t="s">
+        <v>67</v>
       </c>
       <c r="B234" t="s">
         <v>28</v>
@@ -5064,8 +5070,8 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235">
-        <v>2021</v>
+      <c r="A235" t="s">
+        <v>67</v>
       </c>
       <c r="B235" t="s">
         <v>28</v>
@@ -5078,8 +5084,8 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236">
-        <v>2021</v>
+      <c r="A236" t="s">
+        <v>67</v>
       </c>
       <c r="B236" t="s">
         <v>28</v>
@@ -5092,8 +5098,8 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237">
-        <v>2021</v>
+      <c r="A237" t="s">
+        <v>67</v>
       </c>
       <c r="B237" t="s">
         <v>28</v>
@@ -5106,8 +5112,8 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238">
-        <v>2021</v>
+      <c r="A238" t="s">
+        <v>67</v>
       </c>
       <c r="B238" t="s">
         <v>28</v>
@@ -5120,8 +5126,8 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239">
-        <v>2021</v>
+      <c r="A239" t="s">
+        <v>67</v>
       </c>
       <c r="B239" t="s">
         <v>28</v>
@@ -5134,8 +5140,8 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240">
-        <v>2021</v>
+      <c r="A240" t="s">
+        <v>67</v>
       </c>
       <c r="B240" t="s">
         <v>28</v>
@@ -5148,8 +5154,8 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241">
-        <v>2021</v>
+      <c r="A241" t="s">
+        <v>67</v>
       </c>
       <c r="B241" t="s">
         <v>28</v>
@@ -5162,8 +5168,8 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>2021</v>
+      <c r="A242" t="s">
+        <v>67</v>
       </c>
       <c r="B242" t="s">
         <v>29</v>
@@ -5176,8 +5182,8 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243">
-        <v>2021</v>
+      <c r="A243" t="s">
+        <v>67</v>
       </c>
       <c r="B243" t="s">
         <v>29</v>
@@ -5190,8 +5196,8 @@
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244">
-        <v>2021</v>
+      <c r="A244" t="s">
+        <v>67</v>
       </c>
       <c r="B244" t="s">
         <v>29</v>
@@ -5204,8 +5210,8 @@
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245">
-        <v>2021</v>
+      <c r="A245" t="s">
+        <v>67</v>
       </c>
       <c r="B245" t="s">
         <v>29</v>
@@ -5218,8 +5224,8 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246">
-        <v>2021</v>
+      <c r="A246" t="s">
+        <v>67</v>
       </c>
       <c r="B246" t="s">
         <v>29</v>
@@ -5232,8 +5238,8 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247">
-        <v>2021</v>
+      <c r="A247" t="s">
+        <v>67</v>
       </c>
       <c r="B247" t="s">
         <v>29</v>
@@ -5246,8 +5252,8 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248">
-        <v>2021</v>
+      <c r="A248" t="s">
+        <v>67</v>
       </c>
       <c r="B248" t="s">
         <v>29</v>
@@ -5260,8 +5266,8 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249">
-        <v>2021</v>
+      <c r="A249" t="s">
+        <v>67</v>
       </c>
       <c r="B249" t="s">
         <v>29</v>
@@ -5274,8 +5280,8 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250">
-        <v>2021</v>
+      <c r="A250" t="s">
+        <v>67</v>
       </c>
       <c r="B250" t="s">
         <v>29</v>
@@ -5288,8 +5294,8 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251">
-        <v>2021</v>
+      <c r="A251" t="s">
+        <v>67</v>
       </c>
       <c r="B251" t="s">
         <v>29</v>
@@ -5335,8 +5341,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2011</v>
+      <c r="A2" t="s">
+        <v>66</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5349,8 +5355,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
+      <c r="A3" t="s">
+        <v>66</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5363,8 +5369,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2011</v>
+      <c r="A4" t="s">
+        <v>66</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5377,8 +5383,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2011</v>
+      <c r="A5" t="s">
+        <v>66</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5391,8 +5397,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2011</v>
+      <c r="A6" t="s">
+        <v>66</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5405,8 +5411,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2011</v>
+      <c r="A7" t="s">
+        <v>66</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5419,8 +5425,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2011</v>
+      <c r="A8" t="s">
+        <v>66</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5433,8 +5439,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2011</v>
+      <c r="A9" t="s">
+        <v>66</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5447,8 +5453,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2011</v>
+      <c r="A10" t="s">
+        <v>66</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5461,8 +5467,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2011</v>
+      <c r="A11" t="s">
+        <v>66</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5475,8 +5481,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2011</v>
+      <c r="A12" t="s">
+        <v>66</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5489,8 +5495,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2011</v>
+      <c r="A13" t="s">
+        <v>66</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5503,8 +5509,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2011</v>
+      <c r="A14" t="s">
+        <v>66</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5517,8 +5523,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2011</v>
+      <c r="A15" t="s">
+        <v>66</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -5531,8 +5537,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2011</v>
+      <c r="A16" t="s">
+        <v>66</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -5545,8 +5551,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2011</v>
+      <c r="A17" t="s">
+        <v>66</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -5559,8 +5565,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2011</v>
+      <c r="A18" t="s">
+        <v>66</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -5573,8 +5579,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2011</v>
+      <c r="A19" t="s">
+        <v>66</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -5587,8 +5593,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2011</v>
+      <c r="A20" t="s">
+        <v>66</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -5601,8 +5607,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2011</v>
+      <c r="A21" t="s">
+        <v>66</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -5615,8 +5621,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2011</v>
+      <c r="A22" t="s">
+        <v>66</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -5629,8 +5635,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2011</v>
+      <c r="A23" t="s">
+        <v>66</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -5643,8 +5649,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2011</v>
+      <c r="A24" t="s">
+        <v>66</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -5657,8 +5663,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2011</v>
+      <c r="A25" t="s">
+        <v>66</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -5671,8 +5677,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2011</v>
+      <c r="A26" t="s">
+        <v>66</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -5685,8 +5691,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2011</v>
+      <c r="A27" t="s">
+        <v>66</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -5699,8 +5705,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2011</v>
+      <c r="A28" t="s">
+        <v>66</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -5713,8 +5719,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2011</v>
+      <c r="A29" t="s">
+        <v>66</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -5727,8 +5733,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2011</v>
+      <c r="A30" t="s">
+        <v>66</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -5741,8 +5747,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2011</v>
+      <c r="A31" t="s">
+        <v>66</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -5755,8 +5761,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2011</v>
+      <c r="A32" t="s">
+        <v>66</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -5769,8 +5775,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2011</v>
+      <c r="A33" t="s">
+        <v>66</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -5783,8 +5789,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2011</v>
+      <c r="A34" t="s">
+        <v>66</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -5797,8 +5803,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2011</v>
+      <c r="A35" t="s">
+        <v>66</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -5811,8 +5817,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2011</v>
+      <c r="A36" t="s">
+        <v>66</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -5825,8 +5831,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2011</v>
+      <c r="A37" t="s">
+        <v>66</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -5839,8 +5845,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2011</v>
+      <c r="A38" t="s">
+        <v>66</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -5853,8 +5859,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2011</v>
+      <c r="A39" t="s">
+        <v>66</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -5867,8 +5873,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2011</v>
+      <c r="A40" t="s">
+        <v>66</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -5881,8 +5887,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2011</v>
+      <c r="A41" t="s">
+        <v>66</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5895,8 +5901,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2011</v>
+      <c r="A42" t="s">
+        <v>66</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5909,8 +5915,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2011</v>
+      <c r="A43" t="s">
+        <v>66</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5923,8 +5929,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2011</v>
+      <c r="A44" t="s">
+        <v>66</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5937,8 +5943,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2011</v>
+      <c r="A45" t="s">
+        <v>66</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5951,8 +5957,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2011</v>
+      <c r="A46" t="s">
+        <v>66</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5965,8 +5971,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2011</v>
+      <c r="A47" t="s">
+        <v>66</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5979,8 +5985,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2011</v>
+      <c r="A48" t="s">
+        <v>66</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -5993,8 +5999,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2011</v>
+      <c r="A49" t="s">
+        <v>66</v>
       </c>
       <c r="B49">
         <v>4</v>
@@ -6007,8 +6013,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2011</v>
+      <c r="A50" t="s">
+        <v>66</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -6021,8 +6027,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>2011</v>
+      <c r="A51" t="s">
+        <v>66</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -6035,8 +6041,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2011</v>
+      <c r="A52" t="s">
+        <v>66</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -6049,8 +6055,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2011</v>
+      <c r="A53" t="s">
+        <v>66</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -6063,8 +6069,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>2021</v>
+      <c r="A54" t="s">
+        <v>67</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -6077,8 +6083,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>2021</v>
+      <c r="A55" t="s">
+        <v>67</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -6091,8 +6097,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>2021</v>
+      <c r="A56" t="s">
+        <v>67</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6105,8 +6111,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>2021</v>
+      <c r="A57" t="s">
+        <v>67</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -6119,8 +6125,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>2021</v>
+      <c r="A58" t="s">
+        <v>67</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -6133,8 +6139,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2021</v>
+      <c r="A59" t="s">
+        <v>67</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -6147,8 +6153,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>2021</v>
+      <c r="A60" t="s">
+        <v>67</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -6161,8 +6167,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2021</v>
+      <c r="A61" t="s">
+        <v>67</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -6175,8 +6181,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>2021</v>
+      <c r="A62" t="s">
+        <v>67</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -6189,8 +6195,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>2021</v>
+      <c r="A63" t="s">
+        <v>67</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -6203,8 +6209,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2021</v>
+      <c r="A64" t="s">
+        <v>67</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -6217,8 +6223,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>2021</v>
+      <c r="A65" t="s">
+        <v>67</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -6231,8 +6237,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>2021</v>
+      <c r="A66" t="s">
+        <v>67</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -6245,8 +6251,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>2021</v>
+      <c r="A67" t="s">
+        <v>67</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -6259,8 +6265,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>2021</v>
+      <c r="A68" t="s">
+        <v>67</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -6273,8 +6279,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>2021</v>
+      <c r="A69" t="s">
+        <v>67</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -6287,8 +6293,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>2021</v>
+      <c r="A70" t="s">
+        <v>67</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -6301,8 +6307,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>2021</v>
+      <c r="A71" t="s">
+        <v>67</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -6315,8 +6321,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>2021</v>
+      <c r="A72" t="s">
+        <v>67</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -6329,8 +6335,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>2021</v>
+      <c r="A73" t="s">
+        <v>67</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -6343,8 +6349,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>2021</v>
+      <c r="A74" t="s">
+        <v>67</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -6357,8 +6363,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>2021</v>
+      <c r="A75" t="s">
+        <v>67</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -6371,8 +6377,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>2021</v>
+      <c r="A76" t="s">
+        <v>67</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -6385,8 +6391,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>2021</v>
+      <c r="A77" t="s">
+        <v>67</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -6399,8 +6405,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>2021</v>
+      <c r="A78" t="s">
+        <v>67</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -6413,8 +6419,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>2021</v>
+      <c r="A79" t="s">
+        <v>67</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -6427,8 +6433,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>2021</v>
+      <c r="A80" t="s">
+        <v>67</v>
       </c>
       <c r="B80">
         <v>2.5</v>
@@ -6441,8 +6447,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>2021</v>
+      <c r="A81" t="s">
+        <v>67</v>
       </c>
       <c r="B81">
         <v>2.5</v>
@@ -6455,8 +6461,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>2021</v>
+      <c r="A82" t="s">
+        <v>67</v>
       </c>
       <c r="B82">
         <v>2.5</v>
@@ -6469,8 +6475,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>2021</v>
+      <c r="A83" t="s">
+        <v>67</v>
       </c>
       <c r="B83">
         <v>2.5</v>
@@ -6483,8 +6489,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>2021</v>
+      <c r="A84" t="s">
+        <v>67</v>
       </c>
       <c r="B84">
         <v>2.5</v>
@@ -6497,8 +6503,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>2021</v>
+      <c r="A85" t="s">
+        <v>67</v>
       </c>
       <c r="B85">
         <v>2.5</v>
@@ -6511,8 +6517,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>2021</v>
+      <c r="A86" t="s">
+        <v>67</v>
       </c>
       <c r="B86">
         <v>2.5</v>
@@ -6525,8 +6531,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>2021</v>
+      <c r="A87" t="s">
+        <v>67</v>
       </c>
       <c r="B87">
         <v>2.5</v>
@@ -6539,8 +6545,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>2021</v>
+      <c r="A88" t="s">
+        <v>67</v>
       </c>
       <c r="B88">
         <v>2.5</v>
@@ -6553,8 +6559,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>2021</v>
+      <c r="A89" t="s">
+        <v>67</v>
       </c>
       <c r="B89">
         <v>2.5</v>
@@ -6567,8 +6573,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>2021</v>
+      <c r="A90" t="s">
+        <v>67</v>
       </c>
       <c r="B90">
         <v>2.5</v>
@@ -6581,8 +6587,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>2021</v>
+      <c r="A91" t="s">
+        <v>67</v>
       </c>
       <c r="B91">
         <v>2.5</v>
@@ -6595,8 +6601,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>2021</v>
+      <c r="A92" t="s">
+        <v>67</v>
       </c>
       <c r="B92">
         <v>2.5</v>
@@ -6609,8 +6615,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>2021</v>
+      <c r="A93" t="s">
+        <v>67</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -6623,8 +6629,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>2021</v>
+      <c r="A94" t="s">
+        <v>67</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -6637,8 +6643,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>2021</v>
+      <c r="A95" t="s">
+        <v>67</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -6651,8 +6657,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>2021</v>
+      <c r="A96" t="s">
+        <v>67</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -6665,8 +6671,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>2021</v>
+      <c r="A97" t="s">
+        <v>67</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -6679,8 +6685,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>2021</v>
+      <c r="A98" t="s">
+        <v>67</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -6693,8 +6699,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>2021</v>
+      <c r="A99" t="s">
+        <v>67</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -6707,8 +6713,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>2021</v>
+      <c r="A100" t="s">
+        <v>67</v>
       </c>
       <c r="B100">
         <v>3</v>
@@ -6721,8 +6727,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>2021</v>
+      <c r="A101" t="s">
+        <v>67</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -6735,8 +6741,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>2021</v>
+      <c r="A102" t="s">
+        <v>67</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -6749,8 +6755,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>2021</v>
+      <c r="A103" t="s">
+        <v>67</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -6763,8 +6769,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>2021</v>
+      <c r="A104" t="s">
+        <v>67</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -6777,8 +6783,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>2021</v>
+      <c r="A105" t="s">
+        <v>67</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -6791,8 +6797,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>2021</v>
+      <c r="A106" t="s">
+        <v>67</v>
       </c>
       <c r="B106">
         <v>4</v>
@@ -6805,8 +6811,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>2021</v>
+      <c r="A107" t="s">
+        <v>67</v>
       </c>
       <c r="B107">
         <v>4</v>
@@ -6819,8 +6825,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>2021</v>
+      <c r="A108" t="s">
+        <v>67</v>
       </c>
       <c r="B108">
         <v>4</v>
@@ -6833,8 +6839,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>2021</v>
+      <c r="A109" t="s">
+        <v>67</v>
       </c>
       <c r="B109">
         <v>4</v>
@@ -6847,8 +6853,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>2021</v>
+      <c r="A110" t="s">
+        <v>67</v>
       </c>
       <c r="B110">
         <v>4</v>
@@ -6861,8 +6867,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>2021</v>
+      <c r="A111" t="s">
+        <v>67</v>
       </c>
       <c r="B111">
         <v>4</v>
@@ -6875,8 +6881,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>2021</v>
+      <c r="A112" t="s">
+        <v>67</v>
       </c>
       <c r="B112">
         <v>4</v>
@@ -6889,8 +6895,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>2021</v>
+      <c r="A113" t="s">
+        <v>67</v>
       </c>
       <c r="B113">
         <v>4</v>
@@ -6903,8 +6909,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>2021</v>
+      <c r="A114" t="s">
+        <v>67</v>
       </c>
       <c r="B114">
         <v>4</v>
@@ -6917,8 +6923,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>2021</v>
+      <c r="A115" t="s">
+        <v>67</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -6931,8 +6937,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>2021</v>
+      <c r="A116" t="s">
+        <v>67</v>
       </c>
       <c r="B116">
         <v>4</v>
@@ -6945,8 +6951,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117">
-        <v>2021</v>
+      <c r="A117" t="s">
+        <v>67</v>
       </c>
       <c r="B117">
         <v>4</v>
@@ -6959,8 +6965,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>2021</v>
+      <c r="A118" t="s">
+        <v>67</v>
       </c>
       <c r="B118">
         <v>4</v>
@@ -7016,8 +7022,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
+      <c r="A2" t="s">
+        <v>67</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7036,8 +7042,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -7056,8 +7062,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2021</v>
+      <c r="A4" t="s">
+        <v>67</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -7076,8 +7082,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2021</v>
+      <c r="A5" t="s">
+        <v>67</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -7096,8 +7102,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -7116,8 +7122,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -7136,8 +7142,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2021</v>
+      <c r="A8" t="s">
+        <v>67</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -7156,8 +7162,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2021</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7219,8 +7225,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
+      <c r="A2" t="s">
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -7239,8 +7245,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
@@ -7259,8 +7265,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2021</v>
+      <c r="A4" t="s">
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -7279,8 +7285,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2021</v>
+      <c r="A5" t="s">
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -7299,8 +7305,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
@@ -7319,8 +7325,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -7339,8 +7345,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2021</v>
+      <c r="A8" t="s">
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
@@ -7359,8 +7365,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2021</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
@@ -7379,8 +7385,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2021</v>
+      <c r="A10" t="s">
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -7399,8 +7405,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2021</v>
+      <c r="A11" t="s">
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -7419,8 +7425,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2021</v>
+      <c r="A12" t="s">
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>55</v>
@@ -7439,8 +7445,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
+      <c r="A13" t="s">
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
@@ -7459,8 +7465,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2021</v>
+      <c r="A14" t="s">
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
@@ -7479,8 +7485,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2021</v>
+      <c r="A15" t="s">
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
@@ -7499,8 +7505,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2021</v>
+      <c r="A16" t="s">
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>55</v>
@@ -7519,8 +7525,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2021</v>
+      <c r="A17" t="s">
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
@@ -7539,8 +7545,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2021</v>
+      <c r="A18" t="s">
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
@@ -7559,8 +7565,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2021</v>
+      <c r="A19" t="s">
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
@@ -7579,8 +7585,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2021</v>
+      <c r="A20" t="s">
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -7599,8 +7605,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2021</v>
+      <c r="A21" t="s">
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
@@ -7651,8 +7657,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
+      <c r="A2" t="s">
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -7668,8 +7674,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>56</v>
@@ -7685,8 +7691,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2021</v>
+      <c r="A4" t="s">
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
@@ -7702,8 +7708,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2021</v>
+      <c r="A5" t="s">
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -7719,8 +7725,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
@@ -7736,8 +7742,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
@@ -7753,8 +7759,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2021</v>
+      <c r="A8" t="s">
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -7770,8 +7776,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2021</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -7787,8 +7793,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2021</v>
+      <c r="A10" t="s">
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
@@ -7804,8 +7810,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2021</v>
+      <c r="A11" t="s">
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
@@ -7821,8 +7827,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2021</v>
+      <c r="A12" t="s">
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -7838,8 +7844,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
+      <c r="A13" t="s">
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>54</v>
@@ -7864,7 +7870,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7885,8 +7891,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2021</v>
+      <c r="A2" t="s">
+        <v>67</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7896,8 +7902,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
+      <c r="A3" t="s">
+        <v>67</v>
       </c>
       <c r="B3">
         <v>1.0009999999999999</v>
@@ -7907,8 +7913,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2021</v>
+      <c r="A4" t="s">
+        <v>67</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -7918,8 +7924,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2021</v>
+      <c r="A5" t="s">
+        <v>67</v>
       </c>
       <c r="B5">
         <v>2.0009999999999999</v>
@@ -7929,8 +7935,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -7940,8 +7946,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2021</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="B7">
         <v>3.0009999999999999</v>

</xml_diff>